<commit_message>
Updated variable source files for public and research libraries
</commit_message>
<xml_diff>
--- a/data/folk_termer.xlsx
+++ b/data/folk_termer.xlsx
@@ -1896,7 +1896,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1922,26 +1922,21 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF66CC"/>
-        <bgColor rgb="FFFF99CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1978,16 +1973,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2000,73 +1999,13 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF66CC"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F202"/>
@@ -2075,39 +2014,39 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1428571428572"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5714285714286"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5714285714286"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -2126,8 +2065,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -2146,8 +2085,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -2166,8 +2105,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -2186,8 +2125,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
@@ -2206,8 +2145,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -2227,7 +2166,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -2246,8 +2185,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="0" t="s">
@@ -2266,8 +2205,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="0" t="s">
@@ -2286,8 +2225,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="0" t="s">
@@ -2306,8 +2245,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B12" s="0" t="s">
@@ -2326,8 +2265,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B13" s="0" t="s">
@@ -2346,8 +2285,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B14" s="0" t="s">
@@ -2366,8 +2305,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="0" t="s">
@@ -2386,8 +2325,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B16" s="0" t="s">
@@ -2406,8 +2345,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B17" s="0" t="s">
@@ -2426,8 +2365,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B18" s="0" t="s">
@@ -2446,8 +2385,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B19" s="0" t="s">
@@ -2466,8 +2405,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B20" s="0" t="s">
@@ -2486,8 +2425,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B21" s="0" t="s">
@@ -2506,8 +2445,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B22" s="0" t="s">
@@ -2526,8 +2465,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B23" s="0" t="s">
@@ -2546,8 +2485,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B24" s="0" t="s">
@@ -2566,8 +2505,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B25" s="0" t="s">
@@ -2586,8 +2525,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="0" t="s">
@@ -2606,8 +2545,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B27" s="0" t="s">
@@ -2626,8 +2565,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B28" s="0" t="s">
@@ -2646,8 +2585,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B29" s="0" t="s">
@@ -2666,8 +2605,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
         <v>99</v>
       </c>
       <c r="B30" s="0" t="s">
@@ -2686,8 +2625,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B31" s="0" t="s">
@@ -2706,8 +2645,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B32" s="0" t="s">
@@ -2726,8 +2665,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B33" s="0" t="s">
@@ -2746,8 +2685,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B34" s="0" t="s">
@@ -2766,8 +2705,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B35" s="0" t="s">
@@ -2786,8 +2725,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
         <v>117</v>
       </c>
       <c r="B36" s="0" t="s">
@@ -2806,8 +2745,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
         <v>120</v>
       </c>
       <c r="B37" s="0" t="s">
@@ -2826,8 +2765,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="s">
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B38" s="0" t="s">
@@ -2846,8 +2785,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B39" s="0" t="s">
@@ -2866,8 +2805,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B40" s="0" t="s">
@@ -2886,8 +2825,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B41" s="0" t="s">
@@ -2906,8 +2845,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B42" s="0" t="s">
@@ -2926,8 +2865,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
         <v>140</v>
       </c>
       <c r="B43" s="0" t="s">
@@ -2946,8 +2885,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B44" s="0" t="s">
@@ -2966,8 +2905,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="s">
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B45" s="0" t="s">
@@ -2986,8 +2925,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="3" t="s">
         <v>149</v>
       </c>
       <c r="B46" s="0" t="s">
@@ -3006,8 +2945,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="2" t="s">
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="3" t="s">
         <v>152</v>
       </c>
       <c r="B47" s="0" t="s">
@@ -3026,8 +2965,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2" t="s">
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="3" t="s">
         <v>155</v>
       </c>
       <c r="B48" s="0" t="s">
@@ -3046,8 +2985,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="s">
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="3" t="s">
         <v>158</v>
       </c>
       <c r="B49" s="0" t="s">
@@ -3066,8 +3005,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="s">
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="3" t="s">
         <v>161</v>
       </c>
       <c r="B50" s="0" t="s">
@@ -3086,8 +3025,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="s">
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="3" t="s">
         <v>164</v>
       </c>
       <c r="B51" s="0" t="s">
@@ -3106,8 +3045,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2" t="s">
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3" t="s">
         <v>167</v>
       </c>
       <c r="B52" s="0" t="s">
@@ -3126,8 +3065,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="2" t="s">
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="3" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="0" t="s">
@@ -3146,8 +3085,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="s">
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="3" t="s">
         <v>174</v>
       </c>
       <c r="B54" s="0" t="s">
@@ -3166,8 +3105,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="2" t="s">
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="s">
         <v>177</v>
       </c>
       <c r="B55" s="0" t="s">
@@ -3186,8 +3125,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="2" t="s">
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="3" t="s">
         <v>181</v>
       </c>
       <c r="B56" s="0" t="s">
@@ -3206,8 +3145,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="2" t="s">
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="3" t="s">
         <v>185</v>
       </c>
       <c r="B57" s="0" t="s">
@@ -3226,8 +3165,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="2" t="s">
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="3" t="s">
         <v>188</v>
       </c>
       <c r="B58" s="0" t="s">
@@ -3246,8 +3185,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="2" t="s">
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="3" t="s">
         <v>191</v>
       </c>
       <c r="B59" s="0" t="s">
@@ -3266,8 +3205,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="2" t="s">
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="3" t="s">
         <v>194</v>
       </c>
       <c r="B60" s="0" t="s">
@@ -3286,8 +3225,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="s">
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="3" t="s">
         <v>197</v>
       </c>
       <c r="B61" s="0" t="s">
@@ -3306,8 +3245,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="2" t="s">
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="3" t="s">
         <v>200</v>
       </c>
       <c r="B62" s="0" t="s">
@@ -3326,8 +3265,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="2" t="s">
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="3" t="s">
         <v>203</v>
       </c>
       <c r="B63" s="0" t="s">
@@ -3346,8 +3285,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="2" t="s">
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="3" t="s">
         <v>206</v>
       </c>
       <c r="B64" s="0" t="s">
@@ -3366,8 +3305,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="2" t="s">
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="3" t="s">
         <v>209</v>
       </c>
       <c r="B65" s="0" t="s">
@@ -3386,8 +3325,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="2" t="s">
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="3" t="s">
         <v>212</v>
       </c>
       <c r="B66" s="0" t="s">
@@ -3406,8 +3345,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="2" t="s">
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="3" t="s">
         <v>215</v>
       </c>
       <c r="B67" s="0" t="s">
@@ -3426,8 +3365,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="2" t="s">
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="3" t="s">
         <v>218</v>
       </c>
       <c r="B68" s="0" t="s">
@@ -3446,8 +3385,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="2" t="s">
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="3" t="s">
         <v>221</v>
       </c>
       <c r="B69" s="0" t="s">
@@ -3466,8 +3405,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="2" t="s">
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="3" t="s">
         <v>224</v>
       </c>
       <c r="B70" s="0" t="s">
@@ -3486,8 +3425,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2" t="s">
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="3" t="s">
         <v>227</v>
       </c>
       <c r="B71" s="0" t="s">
@@ -3506,8 +3445,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="2" t="s">
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="3" t="s">
         <v>230</v>
       </c>
       <c r="B72" s="0" t="s">
@@ -3526,8 +3465,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="2" t="s">
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="3" t="s">
         <v>233</v>
       </c>
       <c r="B73" s="0" t="s">
@@ -3546,8 +3485,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="2" t="s">
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="3" t="s">
         <v>236</v>
       </c>
       <c r="B74" s="0" t="s">
@@ -3566,8 +3505,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="2" t="s">
+    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="3" t="s">
         <v>239</v>
       </c>
       <c r="B75" s="0" t="s">
@@ -3586,8 +3525,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="2" t="s">
+    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="3" t="s">
         <v>242</v>
       </c>
       <c r="B76" s="0" t="s">
@@ -3606,8 +3545,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="2" t="s">
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="3" t="s">
         <v>245</v>
       </c>
       <c r="B77" s="0" t="s">
@@ -3626,8 +3565,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="2" t="s">
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B78" s="0" t="s">
@@ -3646,8 +3585,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="2" t="s">
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="3" t="s">
         <v>251</v>
       </c>
       <c r="B79" s="0" t="s">
@@ -3666,8 +3605,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="2" t="s">
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="3" t="s">
         <v>254</v>
       </c>
       <c r="B80" s="0" t="s">
@@ -3686,8 +3625,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="2" t="s">
+    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="s">
         <v>257</v>
       </c>
       <c r="B81" s="0" t="s">
@@ -3706,8 +3645,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="2" t="s">
+    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="3" t="s">
         <v>260</v>
       </c>
       <c r="B82" s="0" t="s">
@@ -3726,8 +3665,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="2" t="s">
+    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="3" t="s">
         <v>263</v>
       </c>
       <c r="B83" s="0" t="s">
@@ -3746,8 +3685,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="2" t="s">
+    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="3" t="s">
         <v>266</v>
       </c>
       <c r="B84" s="0" t="s">
@@ -3766,8 +3705,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="2" t="s">
+    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="3" t="s">
         <v>269</v>
       </c>
       <c r="B85" s="0" t="s">
@@ -3786,8 +3725,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="2" t="s">
+    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="3" t="s">
         <v>272</v>
       </c>
       <c r="B86" s="0" t="s">
@@ -3806,8 +3745,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="2" t="s">
+    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="3" t="s">
         <v>275</v>
       </c>
       <c r="B87" s="0" t="s">
@@ -3826,8 +3765,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="2" t="s">
+    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="3" t="s">
         <v>278</v>
       </c>
       <c r="B88" s="0" t="s">
@@ -3846,8 +3785,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="2" t="s">
+    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="3" t="s">
         <v>281</v>
       </c>
       <c r="B89" s="0" t="s">
@@ -3866,8 +3805,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="2" t="s">
+    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="3" t="s">
         <v>284</v>
       </c>
       <c r="B90" s="0" t="s">
@@ -3886,8 +3825,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="2" t="s">
+    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="3" t="s">
         <v>287</v>
       </c>
       <c r="B91" s="0" t="s">
@@ -3906,8 +3845,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="2" t="s">
+    <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="3" t="s">
         <v>290</v>
       </c>
       <c r="B92" s="0" t="s">
@@ -3926,8 +3865,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="2" t="s">
+    <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="3" t="s">
         <v>293</v>
       </c>
       <c r="B93" s="0" t="s">
@@ -3946,8 +3885,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="2" t="s">
+    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="3" t="s">
         <v>296</v>
       </c>
       <c r="B94" s="0" t="s">
@@ -3966,8 +3905,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="2" t="s">
+    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="3" t="s">
         <v>299</v>
       </c>
       <c r="B95" s="0" t="s">
@@ -3986,8 +3925,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="2" t="s">
+    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="3" t="s">
         <v>302</v>
       </c>
       <c r="B96" s="0" t="s">
@@ -4006,8 +3945,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="2" t="s">
+    <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="3" t="s">
         <v>305</v>
       </c>
       <c r="B97" s="0" t="s">
@@ -4026,8 +3965,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="2" t="s">
+    <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="3" t="s">
         <v>308</v>
       </c>
       <c r="B98" s="0" t="s">
@@ -4046,8 +3985,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="2" t="s">
+    <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="3" t="s">
         <v>311</v>
       </c>
       <c r="B99" s="0" t="s">
@@ -4066,8 +4005,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="2" t="s">
+    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="3" t="s">
         <v>314</v>
       </c>
       <c r="B100" s="0" t="s">
@@ -4086,8 +4025,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="2" t="s">
+    <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="3" t="s">
         <v>317</v>
       </c>
       <c r="B101" s="0" t="s">
@@ -4106,8 +4045,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="2" t="s">
+    <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="3" t="s">
         <v>321</v>
       </c>
       <c r="B102" s="0" t="s">
@@ -4126,8 +4065,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="2" t="s">
+    <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="3" t="s">
         <v>324</v>
       </c>
       <c r="B103" s="0" t="s">
@@ -4146,8 +4085,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="2" t="s">
+    <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="3" t="s">
         <v>327</v>
       </c>
       <c r="B104" s="0" t="s">
@@ -4166,8 +4105,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="2" t="s">
+    <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="3" t="s">
         <v>330</v>
       </c>
       <c r="B105" s="0" t="s">
@@ -4186,8 +4125,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="2" t="s">
+    <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="3" t="s">
         <v>334</v>
       </c>
       <c r="B106" s="0" t="s">
@@ -4206,8 +4145,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="2" t="s">
+    <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="3" t="s">
         <v>337</v>
       </c>
       <c r="B107" s="0" t="s">
@@ -4226,8 +4165,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="2" t="s">
+    <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="3" t="s">
         <v>340</v>
       </c>
       <c r="B108" s="0" t="s">
@@ -4246,8 +4185,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="2" t="s">
+    <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="3" t="s">
         <v>343</v>
       </c>
       <c r="B109" s="0" t="s">
@@ -4266,8 +4205,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="2" t="s">
+    <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="3" t="s">
         <v>346</v>
       </c>
       <c r="B110" s="0" t="s">
@@ -4286,8 +4225,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="2" t="s">
+    <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="3" t="s">
         <v>349</v>
       </c>
       <c r="B111" s="0" t="s">
@@ -4306,8 +4245,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="2" t="s">
+    <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="3" t="s">
         <v>352</v>
       </c>
       <c r="B112" s="0" t="s">
@@ -4326,8 +4265,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="2" t="s">
+    <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="3" t="s">
         <v>355</v>
       </c>
       <c r="B113" s="0" t="s">
@@ -4346,8 +4285,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="2" t="s">
+    <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="3" t="s">
         <v>358</v>
       </c>
       <c r="B114" s="0" t="s">
@@ -4366,8 +4305,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="2" t="s">
+    <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="3" t="s">
         <v>361</v>
       </c>
       <c r="B115" s="0" t="s">
@@ -4386,8 +4325,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="2" t="s">
+    <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="3" t="s">
         <v>364</v>
       </c>
       <c r="B116" s="0" t="s">
@@ -4406,8 +4345,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="2" t="s">
+    <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="3" t="s">
         <v>367</v>
       </c>
       <c r="B117" s="0" t="s">
@@ -4426,8 +4365,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="2" t="s">
+    <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="3" t="s">
         <v>370</v>
       </c>
       <c r="B118" s="0" t="s">
@@ -4446,8 +4385,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="2" t="s">
+    <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="3" t="s">
         <v>373</v>
       </c>
       <c r="B119" s="0" t="s">
@@ -4466,8 +4405,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="2" t="s">
+    <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="3" t="s">
         <v>376</v>
       </c>
       <c r="B120" s="0" t="s">
@@ -4486,8 +4425,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="2" t="s">
+    <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="3" t="s">
         <v>379</v>
       </c>
       <c r="B121" s="0" t="s">
@@ -4506,8 +4445,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="2" t="s">
+    <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="3" t="s">
         <v>382</v>
       </c>
       <c r="B122" s="0" t="s">
@@ -4526,8 +4465,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="2" t="s">
+    <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="3" t="s">
         <v>385</v>
       </c>
       <c r="B123" s="0" t="s">
@@ -4546,8 +4485,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="2" t="s">
+    <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="3" t="s">
         <v>388</v>
       </c>
       <c r="B124" s="0" t="s">
@@ -4566,8 +4505,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="2" t="s">
+    <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="3" t="s">
         <v>391</v>
       </c>
       <c r="B125" s="0" t="s">
@@ -4586,8 +4525,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="2" t="s">
+    <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="3" t="s">
         <v>393</v>
       </c>
       <c r="B126" s="0" t="s">
@@ -4606,8 +4545,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="2" t="s">
+    <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="3" t="s">
         <v>395</v>
       </c>
       <c r="B127" s="0" t="s">
@@ -4626,8 +4565,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="2" t="s">
+    <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="3" t="s">
         <v>398</v>
       </c>
       <c r="B128" s="0" t="s">
@@ -4646,8 +4585,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="2" t="s">
+    <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="3" t="s">
         <v>401</v>
       </c>
       <c r="B129" s="0" t="s">
@@ -4666,8 +4605,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="2" t="s">
+    <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="3" t="s">
         <v>403</v>
       </c>
       <c r="B130" s="0" t="s">
@@ -4686,8 +4625,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="2" t="s">
+    <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="3" t="s">
         <v>405</v>
       </c>
       <c r="B131" s="0" t="s">
@@ -4706,8 +4645,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="2" t="s">
+    <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="3" t="s">
         <v>407</v>
       </c>
       <c r="B132" s="0" t="s">
@@ -4726,8 +4665,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="2" t="s">
+    <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="3" t="s">
         <v>410</v>
       </c>
       <c r="B133" s="0" t="s">
@@ -4746,8 +4685,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="2" t="s">
+    <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="3" t="s">
         <v>413</v>
       </c>
       <c r="B134" s="0" t="s">
@@ -4766,8 +4705,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="2" t="s">
+    <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="3" t="s">
         <v>416</v>
       </c>
       <c r="B135" s="0" t="s">
@@ -4786,8 +4725,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="2" t="s">
+    <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="3" t="s">
         <v>419</v>
       </c>
       <c r="B136" s="0" t="s">
@@ -4806,8 +4745,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="2" t="s">
+    <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="3" t="s">
         <v>422</v>
       </c>
       <c r="B137" s="0" t="s">
@@ -4826,8 +4765,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="2" t="s">
+    <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="3" t="s">
         <v>426</v>
       </c>
       <c r="B138" s="0" t="s">
@@ -4846,8 +4785,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="2" t="s">
+    <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="3" t="s">
         <v>429</v>
       </c>
       <c r="B139" s="0" t="s">
@@ -4866,8 +4805,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="2" t="s">
+    <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="3" t="s">
         <v>432</v>
       </c>
       <c r="B140" s="0" t="s">
@@ -4886,8 +4825,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="2" t="s">
+    <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="3" t="s">
         <v>435</v>
       </c>
       <c r="B141" s="0" t="s">
@@ -4906,8 +4845,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="2" t="s">
+    <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="3" t="s">
         <v>438</v>
       </c>
       <c r="B142" s="0" t="s">
@@ -4926,8 +4865,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="2" t="s">
+    <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="3" t="s">
         <v>441</v>
       </c>
       <c r="B143" s="0" t="s">
@@ -4946,8 +4885,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="2" t="s">
+    <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="3" t="s">
         <v>444</v>
       </c>
       <c r="B144" s="0" t="s">
@@ -4966,8 +4905,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="2" t="s">
+    <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="3" t="s">
         <v>447</v>
       </c>
       <c r="B145" s="0" t="s">
@@ -4986,8 +4925,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="2" t="s">
+    <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="3" t="s">
         <v>450</v>
       </c>
       <c r="B146" s="0" t="s">
@@ -5006,8 +4945,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="2" t="s">
+    <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="3" t="s">
         <v>453</v>
       </c>
       <c r="B147" s="0" t="s">
@@ -5026,8 +4965,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="2" t="s">
+    <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="3" t="s">
         <v>456</v>
       </c>
       <c r="B148" s="0" t="s">
@@ -5046,8 +4985,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="2" t="s">
+    <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="3" t="s">
         <v>459</v>
       </c>
       <c r="B149" s="0" t="s">
@@ -5066,8 +5005,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="2" t="s">
+    <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="3" t="s">
         <v>462</v>
       </c>
       <c r="B150" s="0" t="s">
@@ -5086,8 +5025,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="2" t="s">
+    <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="3" t="s">
         <v>465</v>
       </c>
       <c r="B151" s="0" t="s">
@@ -5106,8 +5045,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="2" t="s">
+    <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="3" t="s">
         <v>468</v>
       </c>
       <c r="B152" s="0" t="s">
@@ -5126,8 +5065,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="2" t="s">
+    <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="3" t="s">
         <v>471</v>
       </c>
       <c r="B153" s="0" t="s">
@@ -5146,8 +5085,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="2" t="s">
+    <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="3" t="s">
         <v>474</v>
       </c>
       <c r="B154" s="0" t="s">
@@ -5166,8 +5105,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="2" t="s">
+    <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="3" t="s">
         <v>477</v>
       </c>
       <c r="B155" s="0" t="s">
@@ -5186,8 +5125,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="2" t="s">
+    <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="3" t="s">
         <v>480</v>
       </c>
       <c r="B156" s="0" t="s">
@@ -5206,8 +5145,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="2" t="s">
+    <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="3" t="s">
         <v>483</v>
       </c>
       <c r="B157" s="0" t="s">
@@ -5226,8 +5165,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="2" t="s">
+    <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="3" t="s">
         <v>486</v>
       </c>
       <c r="B158" s="0" t="s">
@@ -5246,8 +5185,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="2" t="s">
+    <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="3" t="s">
         <v>489</v>
       </c>
       <c r="B159" s="0" t="s">
@@ -5266,8 +5205,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="2" t="s">
+    <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="3" t="s">
         <v>492</v>
       </c>
       <c r="B160" s="0" t="s">
@@ -5286,8 +5225,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="2" t="s">
+    <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="3" t="s">
         <v>495</v>
       </c>
       <c r="B161" s="0" t="s">
@@ -5306,8 +5245,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="2" t="s">
+    <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="3" t="s">
         <v>499</v>
       </c>
       <c r="B162" s="0" t="s">
@@ -5326,8 +5265,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="2" t="s">
+    <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="3" t="s">
         <v>502</v>
       </c>
       <c r="B163" s="0" t="s">
@@ -5346,8 +5285,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="2" t="s">
+    <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="3" t="s">
         <v>505</v>
       </c>
       <c r="B164" s="0" t="s">
@@ -5366,8 +5305,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="2" t="s">
+    <row r="165" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="3" t="s">
         <v>508</v>
       </c>
       <c r="B165" s="0" t="s">
@@ -5386,8 +5325,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="2" t="s">
+    <row r="166" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="3" t="s">
         <v>511</v>
       </c>
       <c r="B166" s="0" t="s">
@@ -5406,8 +5345,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="2" t="s">
+    <row r="167" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="3" t="s">
         <v>514</v>
       </c>
       <c r="B167" s="0" t="s">
@@ -5426,8 +5365,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="2" t="s">
+    <row r="168" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="3" t="s">
         <v>517</v>
       </c>
       <c r="B168" s="0" t="s">
@@ -5446,8 +5385,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="2" t="s">
+    <row r="169" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="3" t="s">
         <v>520</v>
       </c>
       <c r="B169" s="0" t="s">
@@ -5466,8 +5405,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="2" t="s">
+    <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="3" t="s">
         <v>523</v>
       </c>
       <c r="B170" s="0" t="s">
@@ -5486,8 +5425,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="2" t="s">
+    <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="3" t="s">
         <v>526</v>
       </c>
       <c r="B171" s="0" t="s">
@@ -5506,8 +5445,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="2" t="s">
+    <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="3" t="s">
         <v>529</v>
       </c>
       <c r="B172" s="0" t="s">
@@ -5526,8 +5465,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="2" t="s">
+    <row r="173" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="3" t="s">
         <v>532</v>
       </c>
       <c r="B173" s="0" t="s">
@@ -5546,8 +5485,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="2" t="s">
+    <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="3" t="s">
         <v>535</v>
       </c>
       <c r="B174" s="0" t="s">
@@ -5566,8 +5505,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="2" t="s">
+    <row r="175" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="3" t="s">
         <v>538</v>
       </c>
       <c r="B175" s="0" t="s">
@@ -5586,8 +5525,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="2" t="s">
+    <row r="176" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="3" t="s">
         <v>541</v>
       </c>
       <c r="B176" s="0" t="s">
@@ -5606,8 +5545,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="2" t="s">
+    <row r="177" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="3" t="s">
         <v>544</v>
       </c>
       <c r="B177" s="0" t="s">
@@ -5626,8 +5565,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="2" t="s">
+    <row r="178" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="3" t="s">
         <v>547</v>
       </c>
       <c r="B178" s="0" t="s">
@@ -5646,8 +5585,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="2" t="s">
+    <row r="179" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="3" t="s">
         <v>550</v>
       </c>
       <c r="B179" s="0" t="s">
@@ -5666,8 +5605,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="2" t="s">
+    <row r="180" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="3" t="s">
         <v>553</v>
       </c>
       <c r="B180" s="0" t="s">
@@ -5686,8 +5625,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="2" t="s">
+    <row r="181" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="3" t="s">
         <v>556</v>
       </c>
       <c r="B181" s="0" t="s">
@@ -5706,8 +5645,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="2" t="s">
+    <row r="182" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="3" t="s">
         <v>559</v>
       </c>
       <c r="B182" s="0" t="s">
@@ -5726,8 +5665,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="2" t="s">
+    <row r="183" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="3" t="s">
         <v>562</v>
       </c>
       <c r="B183" s="0" t="s">
@@ -5746,8 +5685,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="2" t="s">
+    <row r="184" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="3" t="s">
         <v>565</v>
       </c>
       <c r="B184" s="0" t="s">
@@ -5766,8 +5705,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="2" t="s">
+    <row r="185" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="3" t="s">
         <v>568</v>
       </c>
       <c r="B185" s="0" t="s">
@@ -5786,8 +5725,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="2" t="s">
+    <row r="186" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="3" t="s">
         <v>571</v>
       </c>
       <c r="B186" s="0" t="s">
@@ -5806,8 +5745,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="2" t="s">
+    <row r="187" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="3" t="s">
         <v>574</v>
       </c>
       <c r="B187" s="0" t="s">
@@ -5826,8 +5765,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="2" t="s">
+    <row r="188" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="3" t="s">
         <v>577</v>
       </c>
       <c r="B188" s="0" t="s">
@@ -5846,8 +5785,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="2" t="s">
+    <row r="189" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="3" t="s">
         <v>580</v>
       </c>
       <c r="B189" s="0" t="s">
@@ -5866,8 +5805,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="2" t="s">
+    <row r="190" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="3" t="s">
         <v>583</v>
       </c>
       <c r="B190" s="0" t="s">
@@ -5886,8 +5825,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="2" t="s">
+    <row r="191" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="3" t="s">
         <v>586</v>
       </c>
       <c r="B191" s="0" t="s">
@@ -5906,8 +5845,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="2" t="s">
+    <row r="192" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="3" t="s">
         <v>589</v>
       </c>
       <c r="B192" s="0" t="s">
@@ -5926,8 +5865,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="2" t="s">
+    <row r="193" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="3" t="s">
         <v>592</v>
       </c>
       <c r="B193" s="0" t="s">
@@ -5946,8 +5885,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="2" t="s">
+    <row r="194" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="3" t="s">
         <v>595</v>
       </c>
       <c r="B194" s="0" t="s">
@@ -5966,8 +5905,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="2" t="s">
+    <row r="195" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="3" t="s">
         <v>598</v>
       </c>
       <c r="B195" s="0" t="s">
@@ -5986,8 +5925,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="2" t="s">
+    <row r="196" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="3" t="s">
         <v>601</v>
       </c>
       <c r="B196" s="0" t="s">
@@ -6006,8 +5945,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="2" t="s">
+    <row r="197" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="3" t="s">
         <v>604</v>
       </c>
       <c r="B197" s="0" t="s">
@@ -6026,8 +5965,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="2" t="s">
+    <row r="198" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="3" t="s">
         <v>607</v>
       </c>
       <c r="B198" s="0" t="s">
@@ -6046,8 +5985,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="2" t="s">
+    <row r="199" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="3" t="s">
         <v>610</v>
       </c>
       <c r="B199" s="0" t="s">
@@ -6066,8 +6005,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="2" t="s">
+    <row r="200" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="3" t="s">
         <v>614</v>
       </c>
       <c r="B200" s="0" t="s">
@@ -6086,8 +6025,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="2" t="s">
+    <row r="201" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="3" t="s">
         <v>617</v>
       </c>
       <c r="B201" s="0" t="s">
@@ -6106,8 +6045,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="2" t="s">
+    <row r="202" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="3" t="s">
         <v>621</v>
       </c>
       <c r="B202" s="0" t="s">

</xml_diff>